<commit_message>
update benchmarking code and stats for pepmatch
</commit_message>
<xml_diff>
--- a/benchmarking/coronavirus_benchmarking.xlsx
+++ b/benchmarking/coronavirus_benchmarking.xlsx
@@ -148,12 +148,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,162 +174,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>31.707</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>53.643</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>85.35</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>31.547</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>41.754</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>73.301</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>214.712</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.00269174575805664</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>21.323</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>236.038</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.511</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>115.916</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>116.428</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>73.326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.153</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>3.452</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>3.605</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>6.427</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1.83</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>0.77</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>2.6</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>7.377</v>
       </c>
     </row>

</xml_diff>